<commit_message>
check again the function and add questionImage column
</commit_message>
<xml_diff>
--- a/Limitless/LimitLess/Files/standard_files/excel_format.xlsx
+++ b/Limitless/LimitLess/Files/standard_files/excel_format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADSIXPS15\Documents\LimitlessAdmin-update\Limitless\LimitLess\Files\standard_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADSIXPS15\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Upload File" sheetId="1" r:id="rId1"/>
-    <sheet name="Drop down items" sheetId="2" r:id="rId2"/>
+    <sheet name="Drop down items" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Please select a subject</t>
   </si>
@@ -90,9 +90,6 @@
     <t xml:space="preserve">Sub Objective Name </t>
   </si>
   <si>
-    <t xml:space="preserve">Question Content </t>
-  </si>
-  <si>
     <t xml:space="preserve">Question Type </t>
   </si>
   <si>
@@ -157,6 +154,12 @@
   </si>
   <si>
     <t>4 - Image Only</t>
+  </si>
+  <si>
+    <t>Question Content</t>
+  </si>
+  <si>
+    <t>Answer Content</t>
   </si>
 </sst>
 </file>
@@ -514,7 +517,7 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,25 +527,24 @@
     <col min="3" max="3" width="13.77734375" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="15.77734375" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="15" width="21.44140625" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" customWidth="1"/>
-    <col min="17" max="17" width="23" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" customWidth="1"/>
-    <col min="19" max="20" width="21.44140625" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" customWidth="1"/>
-    <col min="22" max="22" width="23" customWidth="1"/>
-    <col min="23" max="23" width="17.6640625" customWidth="1"/>
-    <col min="24" max="25" width="21.44140625" customWidth="1"/>
-    <col min="26" max="26" width="24.44140625" customWidth="1"/>
-    <col min="27" max="27" width="33.77734375" customWidth="1"/>
+    <col min="11" max="12" width="24.44140625" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="15" max="16" width="21.44140625" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" customWidth="1"/>
+    <col min="18" max="18" width="23" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" customWidth="1"/>
+    <col min="20" max="21" width="21.44140625" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" customWidth="1"/>
+    <col min="23" max="23" width="23" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" customWidth="1"/>
+    <col min="25" max="26" width="21.44140625" customWidth="1"/>
+    <col min="28" max="28" width="33.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
@@ -562,67 +564,67 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -630,42 +632,12 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="1041" yWindow="247" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop down items'!$A$1:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop down items'!$B$1:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop down items'!$C$1:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop down items'!$D$1:$D$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop down items'!$E$1:$E$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="1041" yWindow="247" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Drop down items'!$H$1:$H$2</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:O1048576 S2:T1048576 X2:Y1048576 J2:J1048576</xm:sqref>
+          <xm:sqref>O2:P1048576 T2:U1048576 Y2:Z1048576 J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -735,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -744,13 +716,13 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -761,19 +733,19 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -781,24 +753,24 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel format, add question image condition
</commit_message>
<xml_diff>
--- a/Limitless/LimitLess/Files/standard_files/excel_format.xlsx
+++ b/Limitless/LimitLess/Files/standard_files/excel_format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADSIXPS15\Desktop\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADSIXPS15\Documents\LimitlessAdmin-update\Limitless\LimitLess\Files\standard_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="Upload File" sheetId="1" r:id="rId1"/>
-    <sheet name="Drop down items" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Drop down items" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -114,15 +117,6 @@
     <t>3 - sub objective 3</t>
   </si>
   <si>
-    <t>1 - High</t>
-  </si>
-  <si>
-    <t>2 - Medium</t>
-  </si>
-  <si>
-    <t>3 - Low</t>
-  </si>
-  <si>
     <t>Question Is Active</t>
   </si>
   <si>
@@ -144,22 +138,31 @@
     <t>3 - Science</t>
   </si>
   <si>
-    <t>1 - Fill in the Blank</t>
-  </si>
-  <si>
-    <t>2 - Long Strings</t>
-  </si>
-  <si>
-    <t>3 - String with Image</t>
-  </si>
-  <si>
-    <t>4 - Image Only</t>
-  </si>
-  <si>
     <t>Question Content</t>
   </si>
   <si>
     <t>Answer Content</t>
+  </si>
+  <si>
+    <t>Fill in the Blank</t>
+  </si>
+  <si>
+    <t>Long Strings</t>
+  </si>
+  <si>
+    <t>String with Image</t>
+  </si>
+  <si>
+    <t>Image Only</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -195,10 +198,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -215,6 +221,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Upload File"/>
+      <sheetName val="Drop down items"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -514,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,7 +547,7 @@
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
     <col min="3" max="3" width="13.77734375" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="24.44140625" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
@@ -547,7 +568,7 @@
     <col min="28" max="28" width="33.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -564,7 +585,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -576,78 +597,174 @@
         <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="1041" yWindow="247" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="1041" yWindow="247" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Drop down items'!$H$1:$H$2</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:P1048576 T2:U1048576 Y2:Z1048576 J2:J1048576</xm:sqref>
+          <xm:sqref>P2:P1048576 U2:U1048576 J2:J1048576 O2:O1048576 T2:T1048576 Y2:Y1048576 Z2:Z1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Drop down items'!$F$1:$F$4</xm:f>
+            <xm:f>'C:\Users\ADSIXPS15\Desktop\test\[excel_format _withdata (1).xlsx]Drop down items'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>AD4:AE4 K2:K4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop down items'!$F$2:$F$4</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Drop down items'!$G:$G</xm:f>
+            <xm:f>'Drop down items'!$G$2:$G$5</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
@@ -661,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,7 +824,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -719,10 +836,10 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -733,7 +850,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -742,10 +859,10 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -753,7 +870,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -762,15 +879,15 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimize code: answer index
</commit_message>
<xml_diff>
--- a/Limitless/LimitLess/Files/standard_files/excel_format.xlsx
+++ b/Limitless/LimitLess/Files/standard_files/excel_format.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Please select a subject</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>1 - Grammar</t>
-  </si>
-  <si>
-    <t>Attached File</t>
   </si>
   <si>
     <t xml:space="preserve">Organization Name </t>
@@ -535,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,102 +550,99 @@
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="15.77734375" customWidth="1"/>
-    <col min="11" max="12" width="24.44140625" customWidth="1"/>
-    <col min="13" max="13" width="23" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="16" width="21.44140625" customWidth="1"/>
-    <col min="17" max="17" width="19.6640625" customWidth="1"/>
-    <col min="18" max="18" width="23" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" customWidth="1"/>
-    <col min="20" max="21" width="21.44140625" customWidth="1"/>
-    <col min="22" max="22" width="19.6640625" customWidth="1"/>
-    <col min="23" max="23" width="23" customWidth="1"/>
-    <col min="24" max="24" width="17.6640625" customWidth="1"/>
-    <col min="25" max="26" width="21.44140625" customWidth="1"/>
-    <col min="28" max="28" width="33.77734375" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="14" max="15" width="21.44140625" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" customWidth="1"/>
+    <col min="17" max="17" width="23" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" customWidth="1"/>
+    <col min="19" max="20" width="21.44140625" customWidth="1"/>
+    <col min="21" max="21" width="19.6640625" customWidth="1"/>
+    <col min="22" max="22" width="23" customWidth="1"/>
+    <col min="23" max="23" width="17.6640625" customWidth="1"/>
+    <col min="24" max="25" width="21.44140625" customWidth="1"/>
+    <col min="27" max="27" width="33.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="F2" s="2"/>
@@ -676,9 +670,8 @@
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="F3" s="2"/>
@@ -706,9 +699,8 @@
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="F4" s="2"/>
@@ -736,7 +728,6 @@
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -748,13 +739,13 @@
           <x14:formula1>
             <xm:f>'Drop down items'!$H$1:$H$2</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1048576 U2:U1048576 J2:J1048576 O2:O1048576 T2:T1048576 Y2:Y1048576 Z2:Z1048576</xm:sqref>
+          <xm:sqref>O2:O1048576 T2:T1048576 J2:J1048576 N2:N1048576 S2:S1048576 X2:X1048576 Y2:Y1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'C:\Users\ADSIXPS15\Desktop\test\[excel_format _withdata (1).xlsx]Drop down items'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AD4:AE4 K2:K4</xm:sqref>
+          <xm:sqref>AC4:AD4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -824,7 +815,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -833,13 +824,13 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -850,19 +841,19 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -870,24 +861,24 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>